<commit_message>
planilha de cotação teste
</commit_message>
<xml_diff>
--- a/BASE 2024.xlsx
+++ b/BASE 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santosga\Documents\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08985C0F-20D7-452D-A271-E157607BB5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD15CF5-DA73-4904-A57E-6926A99FF6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,14 +1178,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1471,7 +1471,7 @@
   <dimension ref="B2:R341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,7 +1487,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="6"/>
@@ -5777,10 +5777,10 @@
       </c>
     </row>
     <row r="309" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B309" s="5"/>
-      <c r="C309" s="5"/>
-      <c r="D309" s="5"/>
-      <c r="E309" s="5"/>
+      <c r="B309" s="7"/>
+      <c r="C309" s="7"/>
+      <c r="D309" s="7"/>
+      <c r="E309" s="7"/>
     </row>
     <row r="310" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B310" s="6" t="s">
@@ -5835,13 +5835,13 @@
       </c>
     </row>
     <row r="315" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B315" s="5"/>
-      <c r="C315" s="5"/>
-      <c r="D315" s="5"/>
-      <c r="E315" s="5"/>
+      <c r="B315" s="7"/>
+      <c r="C315" s="7"/>
+      <c r="D315" s="7"/>
+      <c r="E315" s="7"/>
     </row>
     <row r="316" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B316" s="7" t="s">
+      <c r="B316" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C316" s="6"/>
@@ -5949,10 +5949,10 @@
       </c>
     </row>
     <row r="325" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B325" s="5"/>
-      <c r="C325" s="5"/>
-      <c r="D325" s="5"/>
-      <c r="E325" s="5"/>
+      <c r="B325" s="7"/>
+      <c r="C325" s="7"/>
+      <c r="D325" s="7"/>
+      <c r="E325" s="7"/>
     </row>
     <row r="326" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B326" s="6" t="s">
@@ -6021,13 +6021,13 @@
       </c>
     </row>
     <row r="332" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B332" s="5"/>
-      <c r="C332" s="5"/>
-      <c r="D332" s="5"/>
-      <c r="E332" s="5"/>
+      <c r="B332" s="7"/>
+      <c r="C332" s="7"/>
+      <c r="D332" s="7"/>
+      <c r="E332" s="7"/>
     </row>
     <row r="333" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B333" s="7" t="s">
+      <c r="B333" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C333" s="6"/>
@@ -6136,12 +6136,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B310:E310"/>
-    <mergeCell ref="B311:E311"/>
-    <mergeCell ref="B309:E309"/>
+    <mergeCell ref="B327:E327"/>
+    <mergeCell ref="B328:E328"/>
+    <mergeCell ref="B333:E333"/>
+    <mergeCell ref="B334:E334"/>
+    <mergeCell ref="B335:E335"/>
+    <mergeCell ref="B332:E332"/>
     <mergeCell ref="B312:E312"/>
     <mergeCell ref="B316:E316"/>
     <mergeCell ref="B317:E317"/>
@@ -6149,13 +6149,14 @@
     <mergeCell ref="B326:E326"/>
     <mergeCell ref="B325:E325"/>
     <mergeCell ref="B315:E315"/>
-    <mergeCell ref="B327:E327"/>
-    <mergeCell ref="B328:E328"/>
-    <mergeCell ref="B333:E333"/>
-    <mergeCell ref="B334:E334"/>
-    <mergeCell ref="B335:E335"/>
-    <mergeCell ref="B332:E332"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B310:E310"/>
+    <mergeCell ref="B311:E311"/>
+    <mergeCell ref="B309:E309"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>